<commit_message>
Deploy: estado local como fuente de verdad
</commit_message>
<xml_diff>
--- a/RESULTADOS T5.xlsx
+++ b/RESULTADOS T5.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\bots\pp_consulta\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5702DDA-B022-4E25-8F17-E36083F84BDC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0C3102C-FFEB-4F8E-9AC7-7C90C6AB1601}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{38F0E9F6-B780-4D16-AEF9-B7D74C50147E}"/>
+    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15720" xr2:uid="{38F0E9F6-B780-4D16-AEF9-B7D74C50147E}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -307,7 +307,7 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -347,6 +347,9 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -678,8 +681,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{63C91A13-D544-4038-9C47-C08B7B768B68}">
   <dimension ref="A1:N132"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="I35" sqref="I35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -780,25 +783,37 @@
         <f>A2</f>
         <v>45915</v>
       </c>
-      <c r="B3" s="6">
+      <c r="B3" s="14">
         <v>3</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="C3" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="D3" s="6" t="s">
+      <c r="D3" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="E3" s="6"/>
-      <c r="F3" s="6"/>
-      <c r="G3" s="6"/>
-      <c r="H3" s="6"/>
-      <c r="I3" s="6"/>
-      <c r="J3" s="6"/>
-      <c r="K3" s="6"/>
-      <c r="L3" s="6"/>
-      <c r="M3" s="6"/>
-      <c r="N3" s="6"/>
+      <c r="E3" s="14">
+        <v>9</v>
+      </c>
+      <c r="F3" s="14">
+        <v>11</v>
+      </c>
+      <c r="G3" s="14">
+        <v>3</v>
+      </c>
+      <c r="H3" s="14">
+        <v>11</v>
+      </c>
+      <c r="I3" s="14">
+        <v>11</v>
+      </c>
+      <c r="J3" s="14">
+        <v>13</v>
+      </c>
+      <c r="K3" s="14"/>
+      <c r="L3" s="14"/>
+      <c r="M3" s="14"/>
+      <c r="N3" s="14"/>
     </row>
     <row r="4" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="13">
@@ -1335,25 +1350,37 @@
         <f>A17</f>
         <v>45922</v>
       </c>
-      <c r="B18" s="6">
+      <c r="B18" s="14">
         <v>18</v>
       </c>
-      <c r="C18" s="6" t="s">
+      <c r="C18" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="D18" s="6" t="s">
+      <c r="D18" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="E18" s="6"/>
-      <c r="F18" s="6"/>
-      <c r="G18" s="6"/>
-      <c r="H18" s="6"/>
-      <c r="I18" s="6"/>
-      <c r="J18" s="6"/>
-      <c r="K18" s="6"/>
-      <c r="L18" s="6"/>
-      <c r="M18" s="6"/>
-      <c r="N18" s="6"/>
+      <c r="E18" s="14">
+        <v>12</v>
+      </c>
+      <c r="F18" s="14">
+        <v>14</v>
+      </c>
+      <c r="G18" s="14">
+        <v>5</v>
+      </c>
+      <c r="H18" s="14">
+        <v>11</v>
+      </c>
+      <c r="I18" s="14">
+        <v>4</v>
+      </c>
+      <c r="J18" s="14">
+        <v>11</v>
+      </c>
+      <c r="K18" s="14"/>
+      <c r="L18" s="14"/>
+      <c r="M18" s="14"/>
+      <c r="N18" s="14"/>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A19" s="12">
@@ -1782,7 +1809,7 @@
         <v>22</v>
       </c>
       <c r="E30" s="3">
-        <v>111</v>
+        <v>11</v>
       </c>
       <c r="F30" s="3">
         <v>6</v>
@@ -1809,25 +1836,37 @@
         <f>A30</f>
         <v>45925</v>
       </c>
-      <c r="B31" s="6">
+      <c r="B31" s="14">
         <v>31</v>
       </c>
-      <c r="C31" s="6" t="s">
+      <c r="C31" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="D31" s="6" t="s">
+      <c r="D31" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="E31" s="6"/>
-      <c r="F31" s="6"/>
-      <c r="G31" s="6"/>
-      <c r="H31" s="6"/>
-      <c r="I31" s="6"/>
-      <c r="J31" s="6"/>
-      <c r="K31" s="6"/>
-      <c r="L31" s="6"/>
-      <c r="M31" s="6"/>
-      <c r="N31" s="6"/>
+      <c r="E31" s="14">
+        <v>10</v>
+      </c>
+      <c r="F31" s="14">
+        <v>12</v>
+      </c>
+      <c r="G31" s="14">
+        <v>7</v>
+      </c>
+      <c r="H31" s="14">
+        <v>11</v>
+      </c>
+      <c r="I31" s="14">
+        <v>7</v>
+      </c>
+      <c r="J31" s="14">
+        <v>11</v>
+      </c>
+      <c r="K31" s="14"/>
+      <c r="L31" s="14"/>
+      <c r="M31" s="14"/>
+      <c r="N31" s="14"/>
     </row>
     <row r="32" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A32" s="13">
@@ -1944,50 +1983,50 @@
         <f>A34</f>
         <v>45929</v>
       </c>
-      <c r="B35" s="8">
+      <c r="B35" s="6">
         <v>35</v>
       </c>
-      <c r="C35" s="3" t="s">
+      <c r="C35" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="D35" s="3" t="s">
+      <c r="D35" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="E35" s="3"/>
-      <c r="F35" s="3"/>
-      <c r="G35" s="3"/>
-      <c r="H35" s="3"/>
-      <c r="I35" s="3"/>
-      <c r="J35" s="3"/>
-      <c r="K35" s="3"/>
-      <c r="L35" s="3"/>
-      <c r="M35" s="3"/>
-      <c r="N35" s="3"/>
+      <c r="E35" s="6"/>
+      <c r="F35" s="6"/>
+      <c r="G35" s="6"/>
+      <c r="H35" s="6"/>
+      <c r="I35" s="6"/>
+      <c r="J35" s="6"/>
+      <c r="K35" s="6"/>
+      <c r="L35" s="6"/>
+      <c r="M35" s="6"/>
+      <c r="N35" s="6"/>
     </row>
     <row r="36" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A36" s="13">
         <f>A35</f>
         <v>45929</v>
       </c>
-      <c r="B36" s="7">
+      <c r="B36" s="9">
         <v>36</v>
       </c>
-      <c r="C36" s="2" t="s">
+      <c r="C36" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="D36" s="2" t="s">
+      <c r="D36" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="E36" s="2"/>
-      <c r="F36" s="2"/>
-      <c r="G36" s="2"/>
-      <c r="H36" s="2"/>
-      <c r="I36" s="2"/>
-      <c r="J36" s="2"/>
-      <c r="K36" s="2"/>
-      <c r="L36" s="2"/>
-      <c r="M36" s="2"/>
-      <c r="N36" s="2"/>
+      <c r="E36" s="9"/>
+      <c r="F36" s="9"/>
+      <c r="G36" s="9"/>
+      <c r="H36" s="9"/>
+      <c r="I36" s="9"/>
+      <c r="J36" s="9"/>
+      <c r="K36" s="9"/>
+      <c r="L36" s="9"/>
+      <c r="M36" s="9"/>
+      <c r="N36" s="9"/>
     </row>
     <row r="37" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A37" s="11">
@@ -2018,25 +2057,25 @@
         <f>A37</f>
         <v>45930</v>
       </c>
-      <c r="B38" s="5">
+      <c r="B38" s="6">
         <v>38</v>
       </c>
-      <c r="C38" s="3" t="s">
+      <c r="C38" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="D38" s="3" t="s">
+      <c r="D38" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="E38" s="3"/>
-      <c r="F38" s="3"/>
-      <c r="G38" s="3"/>
-      <c r="H38" s="3"/>
-      <c r="I38" s="3"/>
-      <c r="J38" s="3"/>
-      <c r="K38" s="3"/>
-      <c r="L38" s="3"/>
-      <c r="M38" s="3"/>
-      <c r="N38" s="3"/>
+      <c r="E38" s="6"/>
+      <c r="F38" s="6"/>
+      <c r="G38" s="6"/>
+      <c r="H38" s="6"/>
+      <c r="I38" s="6"/>
+      <c r="J38" s="6"/>
+      <c r="K38" s="6"/>
+      <c r="L38" s="6"/>
+      <c r="M38" s="6"/>
+      <c r="N38" s="6"/>
     </row>
     <row r="39" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A39" s="12">
@@ -2052,14 +2091,30 @@
       <c r="D39" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="E39" s="3"/>
-      <c r="F39" s="3"/>
-      <c r="G39" s="3"/>
-      <c r="H39" s="3"/>
-      <c r="I39" s="3"/>
-      <c r="J39" s="3"/>
-      <c r="K39" s="3"/>
-      <c r="L39" s="3"/>
+      <c r="E39" s="3">
+        <v>11</v>
+      </c>
+      <c r="F39" s="3">
+        <v>3</v>
+      </c>
+      <c r="G39" s="3">
+        <v>10</v>
+      </c>
+      <c r="H39" s="3">
+        <v>12</v>
+      </c>
+      <c r="I39" s="3">
+        <v>11</v>
+      </c>
+      <c r="J39" s="3">
+        <v>3</v>
+      </c>
+      <c r="K39" s="3">
+        <v>14</v>
+      </c>
+      <c r="L39" s="3">
+        <v>12</v>
+      </c>
       <c r="M39" s="3"/>
       <c r="N39" s="3"/>
     </row>
@@ -2077,12 +2132,24 @@
       <c r="D40" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="E40" s="2"/>
-      <c r="F40" s="2"/>
-      <c r="G40" s="2"/>
-      <c r="H40" s="2"/>
-      <c r="I40" s="2"/>
-      <c r="J40" s="2"/>
+      <c r="E40" s="2">
+        <v>9</v>
+      </c>
+      <c r="F40" s="2">
+        <v>11</v>
+      </c>
+      <c r="G40" s="2">
+        <v>5</v>
+      </c>
+      <c r="H40" s="2">
+        <v>11</v>
+      </c>
+      <c r="I40" s="2">
+        <v>8</v>
+      </c>
+      <c r="J40" s="2">
+        <v>11</v>
+      </c>
       <c r="K40" s="2"/>
       <c r="L40" s="2"/>
       <c r="M40" s="2"/>
@@ -2126,12 +2193,24 @@
       <c r="D42" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="E42" s="3"/>
-      <c r="F42" s="3"/>
-      <c r="G42" s="3"/>
-      <c r="H42" s="3"/>
-      <c r="I42" s="3"/>
-      <c r="J42" s="3"/>
+      <c r="E42" s="3">
+        <v>7</v>
+      </c>
+      <c r="F42" s="3">
+        <v>11</v>
+      </c>
+      <c r="G42" s="3">
+        <v>5</v>
+      </c>
+      <c r="H42" s="3">
+        <v>11</v>
+      </c>
+      <c r="I42" s="3">
+        <v>5</v>
+      </c>
+      <c r="J42" s="3">
+        <v>11</v>
+      </c>
       <c r="K42" s="3"/>
       <c r="L42" s="3"/>
       <c r="M42" s="3"/>
@@ -2142,25 +2221,25 @@
         <f>A42</f>
         <v>45931</v>
       </c>
-      <c r="B43" s="8">
+      <c r="B43" s="6">
         <v>43</v>
       </c>
-      <c r="C43" s="3" t="s">
+      <c r="C43" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="D43" s="3" t="s">
+      <c r="D43" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="E43" s="3"/>
-      <c r="F43" s="3"/>
-      <c r="G43" s="3"/>
-      <c r="H43" s="3"/>
-      <c r="I43" s="3"/>
-      <c r="J43" s="3"/>
-      <c r="K43" s="3"/>
-      <c r="L43" s="3"/>
-      <c r="M43" s="3"/>
-      <c r="N43" s="3"/>
+      <c r="E43" s="6"/>
+      <c r="F43" s="6"/>
+      <c r="G43" s="6"/>
+      <c r="H43" s="6"/>
+      <c r="I43" s="6"/>
+      <c r="J43" s="6"/>
+      <c r="K43" s="6"/>
+      <c r="L43" s="6"/>
+      <c r="M43" s="6"/>
+      <c r="N43" s="6"/>
     </row>
     <row r="44" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A44" s="13">
@@ -2176,14 +2255,30 @@
       <c r="D44" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="E44" s="2"/>
-      <c r="F44" s="2"/>
-      <c r="G44" s="2"/>
-      <c r="H44" s="2"/>
-      <c r="I44" s="2"/>
-      <c r="J44" s="2"/>
-      <c r="K44" s="2"/>
-      <c r="L44" s="2"/>
+      <c r="E44" s="2">
+        <v>11</v>
+      </c>
+      <c r="F44" s="2">
+        <v>4</v>
+      </c>
+      <c r="G44" s="2">
+        <v>11</v>
+      </c>
+      <c r="H44" s="2">
+        <v>5</v>
+      </c>
+      <c r="I44" s="2">
+        <v>6</v>
+      </c>
+      <c r="J44" s="2">
+        <v>11</v>
+      </c>
+      <c r="K44" s="2">
+        <v>11</v>
+      </c>
+      <c r="L44" s="2">
+        <v>8</v>
+      </c>
       <c r="M44" s="2"/>
       <c r="N44" s="2"/>
     </row>

</xml_diff>

<commit_message>
Deploy: arreglando resultados online 8
</commit_message>
<xml_diff>
--- a/RESULTADOS T5.xlsx
+++ b/RESULTADOS T5.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\bots\pp_consulta\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0C3102C-FFEB-4F8E-9AC7-7C90C6AB1601}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2ED55CF-DC12-4E8C-9AB4-9642C16C35A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15720" xr2:uid="{38F0E9F6-B780-4D16-AEF9-B7D74C50147E}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{38F0E9F6-B780-4D16-AEF9-B7D74C50147E}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -681,14 +681,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{63C91A13-D544-4038-9C47-C08B7B768B68}">
   <dimension ref="A1:N132"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="I35" sqref="I35"/>
+    <sheetView tabSelected="1" topLeftCell="A105" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:N132"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="32.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="4" bestFit="1" customWidth="1"/>
     <col min="3" max="4" width="16" bestFit="1" customWidth="1"/>
     <col min="5" max="14" width="5.21875" bestFit="1" customWidth="1"/>
   </cols>
@@ -2057,25 +2057,37 @@
         <f>A37</f>
         <v>45930</v>
       </c>
-      <c r="B38" s="6">
+      <c r="B38" s="8">
         <v>38</v>
       </c>
-      <c r="C38" s="6" t="s">
+      <c r="C38" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="D38" s="6" t="s">
+      <c r="D38" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="E38" s="6"/>
-      <c r="F38" s="6"/>
-      <c r="G38" s="6"/>
-      <c r="H38" s="6"/>
-      <c r="I38" s="6"/>
-      <c r="J38" s="6"/>
-      <c r="K38" s="6"/>
-      <c r="L38" s="6"/>
-      <c r="M38" s="6"/>
-      <c r="N38" s="6"/>
+      <c r="E38" s="3">
+        <v>8</v>
+      </c>
+      <c r="F38" s="3">
+        <v>11</v>
+      </c>
+      <c r="G38" s="3">
+        <v>10</v>
+      </c>
+      <c r="H38" s="3">
+        <v>12</v>
+      </c>
+      <c r="I38" s="3">
+        <v>4</v>
+      </c>
+      <c r="J38" s="3">
+        <v>11</v>
+      </c>
+      <c r="K38" s="3"/>
+      <c r="L38" s="3"/>
+      <c r="M38" s="3"/>
+      <c r="N38" s="3"/>
     </row>
     <row r="39" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A39" s="12">
@@ -2221,25 +2233,37 @@
         <f>A42</f>
         <v>45931</v>
       </c>
-      <c r="B43" s="6">
+      <c r="B43" s="5">
         <v>43</v>
       </c>
-      <c r="C43" s="6" t="s">
+      <c r="C43" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D43" s="6" t="s">
+      <c r="D43" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="E43" s="6"/>
-      <c r="F43" s="6"/>
-      <c r="G43" s="6"/>
-      <c r="H43" s="6"/>
-      <c r="I43" s="6"/>
-      <c r="J43" s="6"/>
-      <c r="K43" s="6"/>
-      <c r="L43" s="6"/>
-      <c r="M43" s="6"/>
-      <c r="N43" s="6"/>
+      <c r="E43" s="3">
+        <v>4</v>
+      </c>
+      <c r="F43" s="3">
+        <v>11</v>
+      </c>
+      <c r="G43" s="3">
+        <v>12</v>
+      </c>
+      <c r="H43" s="3">
+        <v>14</v>
+      </c>
+      <c r="I43" s="3">
+        <v>8</v>
+      </c>
+      <c r="J43" s="3">
+        <v>11</v>
+      </c>
+      <c r="K43" s="3"/>
+      <c r="L43" s="3"/>
+      <c r="M43" s="3"/>
+      <c r="N43" s="3"/>
     </row>
     <row r="44" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A44" s="13">

</xml_diff>

<commit_message>
Deploy: arreglando resultados online 10
</commit_message>
<xml_diff>
--- a/RESULTADOS T5.xlsx
+++ b/RESULTADOS T5.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\bots\pp_consulta\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2ED55CF-DC12-4E8C-9AB4-9642C16C35A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F79AF16-89C5-47E6-8DCC-A02DBF646B80}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{38F0E9F6-B780-4D16-AEF9-B7D74C50147E}"/>
+    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15720" xr2:uid="{38F0E9F6-B780-4D16-AEF9-B7D74C50147E}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -681,7 +681,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{63C91A13-D544-4038-9C47-C08B7B768B68}">
   <dimension ref="A1:N132"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A105" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A103" workbookViewId="0">
       <selection activeCell="B1" sqref="B1:N132"/>
     </sheetView>
   </sheetViews>
@@ -2394,12 +2394,24 @@
       <c r="D48" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="E48" s="2"/>
-      <c r="F48" s="2"/>
-      <c r="G48" s="2"/>
-      <c r="H48" s="2"/>
-      <c r="I48" s="2"/>
-      <c r="J48" s="2"/>
+      <c r="E48" s="2">
+        <v>11</v>
+      </c>
+      <c r="F48" s="2">
+        <v>6</v>
+      </c>
+      <c r="G48" s="2">
+        <v>11</v>
+      </c>
+      <c r="H48" s="2">
+        <v>9</v>
+      </c>
+      <c r="I48" s="2">
+        <v>11</v>
+      </c>
+      <c r="J48" s="2">
+        <v>6</v>
+      </c>
       <c r="K48" s="2"/>
       <c r="L48" s="2"/>
       <c r="M48" s="2"/>
@@ -2443,12 +2455,24 @@
       <c r="D50" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="E50" s="3"/>
-      <c r="F50" s="3"/>
-      <c r="G50" s="3"/>
-      <c r="H50" s="3"/>
-      <c r="I50" s="3"/>
-      <c r="J50" s="3"/>
+      <c r="E50" s="3">
+        <v>11</v>
+      </c>
+      <c r="F50" s="3">
+        <v>5</v>
+      </c>
+      <c r="G50" s="3">
+        <v>11</v>
+      </c>
+      <c r="H50" s="3">
+        <v>4</v>
+      </c>
+      <c r="I50" s="3">
+        <v>12</v>
+      </c>
+      <c r="J50" s="3">
+        <v>10</v>
+      </c>
       <c r="K50" s="3"/>
       <c r="L50" s="3"/>
       <c r="M50" s="3"/>
@@ -2592,12 +2616,24 @@
       <c r="D56" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="E56" s="2"/>
-      <c r="F56" s="2"/>
-      <c r="G56" s="2"/>
-      <c r="H56" s="2"/>
-      <c r="I56" s="2"/>
-      <c r="J56" s="2"/>
+      <c r="E56" s="2">
+        <v>11</v>
+      </c>
+      <c r="F56" s="2">
+        <v>6</v>
+      </c>
+      <c r="G56" s="2">
+        <v>11</v>
+      </c>
+      <c r="H56" s="2">
+        <v>4</v>
+      </c>
+      <c r="I56" s="2">
+        <v>11</v>
+      </c>
+      <c r="J56" s="2">
+        <v>7</v>
+      </c>
       <c r="K56" s="2"/>
       <c r="L56" s="2"/>
       <c r="M56" s="2"/>

</xml_diff>